<commit_message>
Fixed fuckups & updated Games 2022
</commit_message>
<xml_diff>
--- a/spreadsheets/Games.xlsx
+++ b/spreadsheets/Games.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8130" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8130" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="2019" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="315">
   <si>
     <t>Nier: Automata</t>
   </si>
@@ -1692,7 +1692,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2162,6 +2162,9 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
@@ -2180,9 +2183,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2190,6 +2190,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2714,11 +2717,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2012926832"/>
-        <c:axId val="2012925744"/>
+        <c:axId val="-1381972208"/>
+        <c:axId val="-1381968944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2012926832"/>
+        <c:axId val="-1381972208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2799,7 +2802,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2012925744"/>
+        <c:crossAx val="-1381968944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2807,7 +2810,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2012925744"/>
+        <c:axId val="-1381968944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2909,7 +2912,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2012926832"/>
+        <c:crossAx val="-1381972208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3281,11 +3284,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2012912144"/>
-        <c:axId val="2012912688"/>
+        <c:axId val="-1381976016"/>
+        <c:axId val="-1381971664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2012912144"/>
+        <c:axId val="-1381976016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3328,7 +3331,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2012912688"/>
+        <c:crossAx val="-1381971664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3336,7 +3339,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2012912688"/>
+        <c:axId val="-1381971664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3387,7 +3390,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2012912144"/>
+        <c:crossAx val="-1381976016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3774,11 +3777,11 @@
         </c:dLbls>
         <c:gapWidth val="444"/>
         <c:overlap val="-90"/>
-        <c:axId val="2014545376"/>
-        <c:axId val="2014541024"/>
+        <c:axId val="-1381969488"/>
+        <c:axId val="-1381968400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2014545376"/>
+        <c:axId val="-1381969488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3835,7 +3838,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2014541024"/>
+        <c:crossAx val="-1381968400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3843,7 +3846,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2014541024"/>
+        <c:axId val="-1381968400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3853,7 +3856,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2014545376"/>
+        <c:crossAx val="-1381969488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4167,11 +4170,11 @@
         </c:dLbls>
         <c:gapWidth val="50"/>
         <c:overlap val="100"/>
-        <c:axId val="2014541568"/>
-        <c:axId val="2014535584"/>
+        <c:axId val="-1186767312"/>
+        <c:axId val="-1186756432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2014541568"/>
+        <c:axId val="-1186767312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4216,7 +4219,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2014535584"/>
+        <c:crossAx val="-1186756432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4224,7 +4227,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2014535584"/>
+        <c:axId val="-1186756432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4274,7 +4277,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2014541568"/>
+        <c:crossAx val="-1186767312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.5"/>
@@ -4412,6 +4415,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4501,6 +4505,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4710,11 +4715,11 @@
         </c:dLbls>
         <c:gapWidth val="444"/>
         <c:overlap val="-90"/>
-        <c:axId val="2014539392"/>
-        <c:axId val="2014542112"/>
+        <c:axId val="-1186771120"/>
+        <c:axId val="-1186758608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2014539392"/>
+        <c:axId val="-1186771120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4771,7 +4776,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2014542112"/>
+        <c:crossAx val="-1186758608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4779,7 +4784,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2014542112"/>
+        <c:axId val="-1186758608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4789,7 +4794,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2014539392"/>
+        <c:crossAx val="-1186771120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5055,11 +5060,11 @@
         </c:dLbls>
         <c:gapWidth val="50"/>
         <c:overlap val="100"/>
-        <c:axId val="2014542656"/>
-        <c:axId val="2014534496"/>
+        <c:axId val="-1186760240"/>
+        <c:axId val="-1186757520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2014542656"/>
+        <c:axId val="-1186760240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5104,7 +5109,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2014534496"/>
+        <c:crossAx val="-1186757520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5112,7 +5117,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2014534496"/>
+        <c:axId val="-1186757520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5162,7 +5167,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2014542656"/>
+        <c:crossAx val="-1186760240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.5"/>
@@ -15042,7 +15047,7 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:AY296"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
@@ -15210,7 +15215,7 @@
         <v>4.197916666666667</v>
       </c>
       <c r="H3" s="8"/>
-      <c r="I3" s="160" t="s">
+      <c r="I3" s="161" t="s">
         <v>124</v>
       </c>
       <c r="J3" s="84" t="s">
@@ -15281,7 +15286,7 @@
         <v>0.30138888888888887</v>
       </c>
       <c r="H4" s="8"/>
-      <c r="I4" s="161"/>
+      <c r="I4" s="162"/>
       <c r="J4" s="57" t="s">
         <v>133</v>
       </c>
@@ -15350,7 +15355,7 @@
         <v>0.2076388888888889</v>
       </c>
       <c r="H5" s="8"/>
-      <c r="I5" s="161"/>
+      <c r="I5" s="162"/>
       <c r="J5" s="77" t="s">
         <v>138</v>
       </c>
@@ -15419,7 +15424,7 @@
         <v>1.2437499999999999</v>
       </c>
       <c r="H6" s="8"/>
-      <c r="I6" s="161"/>
+      <c r="I6" s="162"/>
       <c r="J6" s="57" t="s">
         <v>135</v>
       </c>
@@ -15488,7 +15493,7 @@
         <v>0.27916666666666667</v>
       </c>
       <c r="H7" s="8"/>
-      <c r="I7" s="161"/>
+      <c r="I7" s="162"/>
       <c r="J7" s="77" t="s">
         <v>142</v>
       </c>
@@ -15557,7 +15562,7 @@
         <v>6.1111111111111116E-2</v>
       </c>
       <c r="H8" s="8"/>
-      <c r="I8" s="161"/>
+      <c r="I8" s="162"/>
       <c r="J8" s="57" t="s">
         <v>143</v>
       </c>
@@ -15626,7 +15631,7 @@
         <v>0.11180555555555556</v>
       </c>
       <c r="H9" s="8"/>
-      <c r="I9" s="160" t="s">
+      <c r="I9" s="161" t="s">
         <v>125</v>
       </c>
       <c r="J9" s="75" t="s">
@@ -15697,7 +15702,7 @@
         <v>0.19027777777777777</v>
       </c>
       <c r="H10" s="8"/>
-      <c r="I10" s="161"/>
+      <c r="I10" s="162"/>
       <c r="J10" s="57" t="s">
         <v>133</v>
       </c>
@@ -15766,7 +15771,7 @@
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="H11" s="8"/>
-      <c r="I11" s="161"/>
+      <c r="I11" s="162"/>
       <c r="J11" s="77" t="s">
         <v>138</v>
       </c>
@@ -15835,7 +15840,7 @@
         <v>1.7097222222222221</v>
       </c>
       <c r="H12" s="8"/>
-      <c r="I12" s="161"/>
+      <c r="I12" s="162"/>
       <c r="J12" s="57" t="s">
         <v>135</v>
       </c>
@@ -15904,7 +15909,7 @@
         <v>0.15972222222222224</v>
       </c>
       <c r="H13" s="8"/>
-      <c r="I13" s="161"/>
+      <c r="I13" s="162"/>
       <c r="J13" s="77" t="s">
         <v>147</v>
       </c>
@@ -15973,7 +15978,7 @@
         <v>0.14722222222222223</v>
       </c>
       <c r="H14" s="8"/>
-      <c r="I14" s="160" t="s">
+      <c r="I14" s="161" t="s">
         <v>126</v>
       </c>
       <c r="J14" s="11" t="s">
@@ -16044,7 +16049,7 @@
         <v>0.59652777777777777</v>
       </c>
       <c r="H15" s="8"/>
-      <c r="I15" s="161"/>
+      <c r="I15" s="162"/>
       <c r="J15" s="77" t="s">
         <v>133</v>
       </c>
@@ -16113,7 +16118,7 @@
         <v>14</v>
       </c>
       <c r="H16" s="8"/>
-      <c r="I16" s="161"/>
+      <c r="I16" s="162"/>
       <c r="J16" s="57" t="s">
         <v>138</v>
       </c>
@@ -16182,7 +16187,7 @@
         <v>14</v>
       </c>
       <c r="H17" s="8"/>
-      <c r="I17" s="161"/>
+      <c r="I17" s="162"/>
       <c r="J17" s="77" t="s">
         <v>135</v>
       </c>
@@ -16251,7 +16256,7 @@
         <v>0.24583333333333335</v>
       </c>
       <c r="H18" s="8"/>
-      <c r="I18" s="161"/>
+      <c r="I18" s="162"/>
       <c r="J18" s="57" t="s">
         <v>150</v>
       </c>
@@ -16320,7 +16325,7 @@
         <v>0.49513888888888885</v>
       </c>
       <c r="H19" s="8"/>
-      <c r="I19" s="162"/>
+      <c r="I19" s="163"/>
       <c r="J19" s="80" t="s">
         <v>156</v>
       </c>
@@ -16389,7 +16394,7 @@
         <v>0.20972222222222223</v>
       </c>
       <c r="H20" s="8"/>
-      <c r="I20" s="160" t="s">
+      <c r="I20" s="161" t="s">
         <v>149</v>
       </c>
       <c r="J20" s="11" t="s">
@@ -16460,7 +16465,7 @@
         <v>0.25486111111111109</v>
       </c>
       <c r="H21" s="8"/>
-      <c r="I21" s="162"/>
+      <c r="I21" s="163"/>
       <c r="J21" s="80" t="s">
         <v>147</v>
       </c>
@@ -16539,7 +16544,7 @@
         <v>0.26666666666666666</v>
       </c>
       <c r="H22" s="8"/>
-      <c r="I22" s="161" t="s">
+      <c r="I22" s="162" t="s">
         <v>167</v>
       </c>
       <c r="J22" s="57" t="s">
@@ -16622,7 +16627,7 @@
         <v>0.26944444444444443</v>
       </c>
       <c r="H23" s="8"/>
-      <c r="I23" s="161"/>
+      <c r="I23" s="162"/>
       <c r="J23" s="84" t="s">
         <v>175</v>
       </c>
@@ -16703,7 +16708,7 @@
         <v>0.3263888888888889</v>
       </c>
       <c r="H24" s="40"/>
-      <c r="I24" s="161"/>
+      <c r="I24" s="162"/>
       <c r="J24" s="57" t="s">
         <v>169</v>
       </c>
@@ -16784,7 +16789,7 @@
         <v>0.32847222222222222</v>
       </c>
       <c r="H25" s="41"/>
-      <c r="I25" s="161"/>
+      <c r="I25" s="162"/>
       <c r="J25" s="77" t="s">
         <v>147</v>
       </c>
@@ -16865,7 +16870,7 @@
         <v>0.67013888888888884</v>
       </c>
       <c r="H26" s="41"/>
-      <c r="I26" s="162"/>
+      <c r="I26" s="163"/>
       <c r="J26" s="12" t="s">
         <v>168</v>
       </c>
@@ -16946,7 +16951,7 @@
         <v>0.11180555555555556</v>
       </c>
       <c r="H27" s="41"/>
-      <c r="I27" s="160" t="s">
+      <c r="I27" s="161" t="s">
         <v>177</v>
       </c>
       <c r="J27" s="77" t="s">
@@ -17029,7 +17034,7 @@
         <v>0.22291666666666665</v>
       </c>
       <c r="H28" s="41"/>
-      <c r="I28" s="161"/>
+      <c r="I28" s="162"/>
       <c r="J28" s="105" t="s">
         <v>169</v>
       </c>
@@ -17110,7 +17115,7 @@
         <v>0.13194444444444445</v>
       </c>
       <c r="H29" s="41"/>
-      <c r="I29" s="161"/>
+      <c r="I29" s="162"/>
       <c r="J29" s="77" t="s">
         <v>30</v>
       </c>
@@ -17191,7 +17196,7 @@
         <v>14</v>
       </c>
       <c r="H30" s="41"/>
-      <c r="I30" s="161"/>
+      <c r="I30" s="162"/>
       <c r="J30" s="105" t="s">
         <v>142</v>
       </c>
@@ -17272,7 +17277,7 @@
         <v>0.43888888888888888</v>
       </c>
       <c r="H31" s="41"/>
-      <c r="I31" s="162"/>
+      <c r="I31" s="163"/>
       <c r="J31" s="77" t="s">
         <v>147</v>
       </c>
@@ -17353,7 +17358,7 @@
         <v>0.42083333333333334</v>
       </c>
       <c r="H32" s="41"/>
-      <c r="I32" s="160" t="s">
+      <c r="I32" s="161" t="s">
         <v>190</v>
       </c>
       <c r="J32" s="111" t="s">
@@ -17436,7 +17441,7 @@
         <v>2.7097222222222221</v>
       </c>
       <c r="H33" s="41"/>
-      <c r="I33" s="161"/>
+      <c r="I33" s="162"/>
       <c r="J33" s="77" t="s">
         <v>185</v>
       </c>
@@ -17519,7 +17524,7 @@
         <v>14</v>
       </c>
       <c r="H34" s="41"/>
-      <c r="I34" s="161"/>
+      <c r="I34" s="162"/>
       <c r="J34" s="57" t="s">
         <v>205</v>
       </c>
@@ -17599,7 +17604,7 @@
         <v>0.11041666666666666</v>
       </c>
       <c r="H35" s="41"/>
-      <c r="I35" s="161"/>
+      <c r="I35" s="162"/>
       <c r="J35" s="84" t="s">
         <v>204</v>
       </c>
@@ -17668,7 +17673,7 @@
         <v>0.37083333333333335</v>
       </c>
       <c r="H36" s="41"/>
-      <c r="I36" s="161"/>
+      <c r="I36" s="162"/>
       <c r="J36" s="57" t="s">
         <v>147</v>
       </c>
@@ -17676,9 +17681,9 @@
         <v>4.5138888888888888E-2</v>
       </c>
       <c r="L36" s="41"/>
-      <c r="M36" s="163"/>
-      <c r="N36" s="163"/>
-      <c r="O36" s="163"/>
+      <c r="M36" s="157"/>
+      <c r="N36" s="157"/>
+      <c r="O36" s="157"/>
       <c r="P36" s="129"/>
       <c r="Q36" s="43"/>
       <c r="R36" s="43"/>
@@ -17737,7 +17742,7 @@
         <v>0.80694444444444446</v>
       </c>
       <c r="H37" s="41"/>
-      <c r="I37" s="161"/>
+      <c r="I37" s="162"/>
       <c r="J37" s="84" t="s">
         <v>202</v>
       </c>
@@ -17745,9 +17750,9 @@
         <v>7.7777777777777779E-2</v>
       </c>
       <c r="L37" s="41"/>
-      <c r="M37" s="163"/>
-      <c r="N37" s="163"/>
-      <c r="O37" s="163"/>
+      <c r="M37" s="157"/>
+      <c r="N37" s="157"/>
+      <c r="O37" s="157"/>
       <c r="P37" s="129"/>
       <c r="Q37" s="43"/>
       <c r="R37" s="43"/>
@@ -17806,7 +17811,7 @@
         <v>9.1666666666666674E-2</v>
       </c>
       <c r="H38" s="41"/>
-      <c r="I38" s="162"/>
+      <c r="I38" s="163"/>
       <c r="J38" s="12" t="s">
         <v>208</v>
       </c>
@@ -17814,9 +17819,9 @@
         <v>9.1666666666666674E-2</v>
       </c>
       <c r="L38" s="41"/>
-      <c r="M38" s="163"/>
-      <c r="N38" s="163"/>
-      <c r="O38" s="163"/>
+      <c r="M38" s="157"/>
+      <c r="N38" s="157"/>
+      <c r="O38" s="157"/>
       <c r="P38" s="129"/>
       <c r="Q38" s="43"/>
       <c r="R38" s="43"/>
@@ -17863,7 +17868,7 @@
       <c r="F39" s="31"/>
       <c r="G39" s="64"/>
       <c r="H39" s="41"/>
-      <c r="I39" s="160" t="s">
+      <c r="I39" s="161" t="s">
         <v>217</v>
       </c>
       <c r="J39" s="120" t="s">
@@ -17873,9 +17878,9 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="L39" s="41"/>
-      <c r="M39" s="163"/>
-      <c r="N39" s="163"/>
-      <c r="O39" s="163"/>
+      <c r="M39" s="157"/>
+      <c r="N39" s="157"/>
+      <c r="O39" s="157"/>
       <c r="P39" s="128"/>
       <c r="Q39" s="43"/>
       <c r="R39" s="43"/>
@@ -17922,7 +17927,7 @@
       <c r="F40" s="40"/>
       <c r="G40" s="65"/>
       <c r="H40" s="41"/>
-      <c r="I40" s="161"/>
+      <c r="I40" s="162"/>
       <c r="J40" s="117" t="s">
         <v>218</v>
       </c>
@@ -17930,9 +17935,9 @@
         <v>0.3666666666666667</v>
       </c>
       <c r="L40" s="41"/>
-      <c r="M40" s="163"/>
-      <c r="N40" s="163"/>
-      <c r="O40" s="163"/>
+      <c r="M40" s="157"/>
+      <c r="N40" s="157"/>
+      <c r="O40" s="157"/>
       <c r="P40" s="128"/>
       <c r="Q40" s="43"/>
       <c r="R40" s="43"/>
@@ -17978,7 +17983,7 @@
       <c r="F41" s="31"/>
       <c r="G41" s="64"/>
       <c r="H41" s="41"/>
-      <c r="I41" s="161"/>
+      <c r="I41" s="162"/>
       <c r="J41" s="116" t="s">
         <v>185</v>
       </c>
@@ -17986,9 +17991,9 @@
         <v>0.53333333333333333</v>
       </c>
       <c r="L41" s="41"/>
-      <c r="M41" s="163"/>
-      <c r="N41" s="163"/>
-      <c r="O41" s="163"/>
+      <c r="M41" s="157"/>
+      <c r="N41" s="157"/>
+      <c r="O41" s="157"/>
       <c r="P41" s="128"/>
       <c r="Q41" s="43"/>
       <c r="R41" s="43"/>
@@ -18035,7 +18040,7 @@
       <c r="F42" s="31"/>
       <c r="G42" s="64"/>
       <c r="H42" s="41"/>
-      <c r="I42" s="161"/>
+      <c r="I42" s="162"/>
       <c r="J42" s="118" t="s">
         <v>142</v>
       </c>
@@ -18092,7 +18097,7 @@
       <c r="F43" s="41"/>
       <c r="G43" s="66"/>
       <c r="H43" s="41"/>
-      <c r="I43" s="161"/>
+      <c r="I43" s="162"/>
       <c r="J43" s="116" t="s">
         <v>220</v>
       </c>
@@ -18149,7 +18154,7 @@
       <c r="F44" s="41"/>
       <c r="G44" s="66"/>
       <c r="H44" s="41"/>
-      <c r="I44" s="161"/>
+      <c r="I44" s="162"/>
       <c r="J44" s="117" t="s">
         <v>221</v>
       </c>
@@ -18206,7 +18211,7 @@
       <c r="F45" s="41"/>
       <c r="G45" s="66"/>
       <c r="H45" s="41"/>
-      <c r="I45" s="162"/>
+      <c r="I45" s="163"/>
       <c r="J45" s="119" t="s">
         <v>147</v>
       </c>
@@ -18263,7 +18268,7 @@
       <c r="F46" s="41"/>
       <c r="G46" s="66"/>
       <c r="H46" s="41"/>
-      <c r="I46" s="157" t="s">
+      <c r="I46" s="158" t="s">
         <v>225</v>
       </c>
       <c r="J46" s="123" t="s">
@@ -18322,7 +18327,7 @@
       <c r="F47" s="41"/>
       <c r="G47" s="66"/>
       <c r="H47" s="41"/>
-      <c r="I47" s="158"/>
+      <c r="I47" s="159"/>
       <c r="J47" s="84" t="s">
         <v>185</v>
       </c>
@@ -18379,7 +18384,7 @@
       <c r="F48" s="41"/>
       <c r="G48" s="66"/>
       <c r="H48" s="41"/>
-      <c r="I48" s="158"/>
+      <c r="I48" s="159"/>
       <c r="J48" s="105" t="s">
         <v>142</v>
       </c>
@@ -18436,7 +18441,7 @@
       <c r="F49" s="41"/>
       <c r="G49" s="66"/>
       <c r="H49" s="41"/>
-      <c r="I49" s="159"/>
+      <c r="I49" s="160"/>
       <c r="J49" s="124" t="s">
         <v>221</v>
       </c>
@@ -18493,7 +18498,7 @@
       <c r="F50" s="41"/>
       <c r="G50" s="41"/>
       <c r="H50" s="41"/>
-      <c r="I50" s="157" t="s">
+      <c r="I50" s="158" t="s">
         <v>240</v>
       </c>
       <c r="J50" s="125" t="s">
@@ -18552,7 +18557,7 @@
       <c r="F51" s="41"/>
       <c r="G51" s="41"/>
       <c r="H51" s="41"/>
-      <c r="I51" s="158"/>
+      <c r="I51" s="159"/>
       <c r="J51" s="126" t="s">
         <v>185</v>
       </c>
@@ -18609,7 +18614,7 @@
       <c r="F52" s="41"/>
       <c r="G52" s="41"/>
       <c r="H52" s="41"/>
-      <c r="I52" s="158"/>
+      <c r="I52" s="159"/>
       <c r="J52" s="118" t="s">
         <v>243</v>
       </c>
@@ -18666,7 +18671,7 @@
       <c r="F53" s="41"/>
       <c r="G53" s="41"/>
       <c r="H53" s="41"/>
-      <c r="I53" s="159"/>
+      <c r="I53" s="160"/>
       <c r="J53" s="119" t="s">
         <v>219</v>
       </c>
@@ -18723,7 +18728,7 @@
       <c r="F54" s="41"/>
       <c r="G54" s="41"/>
       <c r="H54" s="41"/>
-      <c r="I54" s="157" t="s">
+      <c r="I54" s="158" t="s">
         <v>251</v>
       </c>
       <c r="J54" s="125" t="s">
@@ -18782,7 +18787,7 @@
       <c r="F55" s="41"/>
       <c r="G55" s="41"/>
       <c r="H55" s="41"/>
-      <c r="I55" s="158"/>
+      <c r="I55" s="159"/>
       <c r="J55" s="126" t="s">
         <v>250</v>
       </c>
@@ -18839,7 +18844,7 @@
       <c r="F56" s="41"/>
       <c r="G56" s="41"/>
       <c r="H56" s="41"/>
-      <c r="I56" s="158"/>
+      <c r="I56" s="159"/>
       <c r="J56" s="118" t="s">
         <v>30</v>
       </c>
@@ -18896,7 +18901,7 @@
       <c r="F57" s="41"/>
       <c r="G57" s="41"/>
       <c r="H57" s="41"/>
-      <c r="I57" s="159"/>
+      <c r="I57" s="160"/>
       <c r="J57" s="119" t="s">
         <v>205</v>
       </c>
@@ -18953,7 +18958,7 @@
       <c r="F58" s="41"/>
       <c r="G58" s="41"/>
       <c r="H58" s="41"/>
-      <c r="I58" s="157" t="s">
+      <c r="I58" s="158" t="s">
         <v>254</v>
       </c>
       <c r="J58" s="125" t="s">
@@ -19012,7 +19017,7 @@
       <c r="F59" s="41"/>
       <c r="G59" s="41"/>
       <c r="H59" s="41"/>
-      <c r="I59" s="158"/>
+      <c r="I59" s="159"/>
       <c r="J59" s="126" t="s">
         <v>243</v>
       </c>
@@ -19069,7 +19074,7 @@
       <c r="F60" s="41"/>
       <c r="G60" s="41"/>
       <c r="H60" s="41"/>
-      <c r="I60" s="158"/>
+      <c r="I60" s="159"/>
       <c r="J60" s="118" t="s">
         <v>250</v>
       </c>
@@ -19126,7 +19131,7 @@
       <c r="F61" s="41"/>
       <c r="G61" s="41"/>
       <c r="H61" s="41"/>
-      <c r="I61" s="158"/>
+      <c r="I61" s="159"/>
       <c r="J61" s="126" t="s">
         <v>253</v>
       </c>
@@ -19183,7 +19188,7 @@
       <c r="F62" s="41"/>
       <c r="G62" s="41"/>
       <c r="H62" s="41"/>
-      <c r="I62" s="158"/>
+      <c r="I62" s="159"/>
       <c r="J62" s="118" t="s">
         <v>30</v>
       </c>
@@ -19240,7 +19245,7 @@
       <c r="F63" s="41"/>
       <c r="G63" s="41"/>
       <c r="H63" s="41"/>
-      <c r="I63" s="159"/>
+      <c r="I63" s="160"/>
       <c r="J63" s="119" t="s">
         <v>205</v>
       </c>
@@ -24894,12 +24899,6 @@
     <sortCondition ref="J33"/>
   </sortState>
   <mergeCells count="18">
-    <mergeCell ref="M41:O41"/>
-    <mergeCell ref="M40:O40"/>
-    <mergeCell ref="M37:O37"/>
-    <mergeCell ref="M36:O36"/>
-    <mergeCell ref="M38:O38"/>
-    <mergeCell ref="M39:O39"/>
     <mergeCell ref="I58:I63"/>
     <mergeCell ref="I54:I57"/>
     <mergeCell ref="I50:I53"/>
@@ -24912,6 +24911,12 @@
     <mergeCell ref="I32:I38"/>
     <mergeCell ref="I27:I31"/>
     <mergeCell ref="I14:I19"/>
+    <mergeCell ref="M41:O41"/>
+    <mergeCell ref="M40:O40"/>
+    <mergeCell ref="M37:O37"/>
+    <mergeCell ref="M36:O36"/>
+    <mergeCell ref="M38:O38"/>
+    <mergeCell ref="M39:O39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -24927,8 +24932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V153"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -25439,11 +25444,11 @@
       <c r="F13" s="78"/>
       <c r="G13" s="79"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="117"/>
-      <c r="J13" s="140"/>
-      <c r="K13" s="145"/>
-      <c r="L13" s="57"/>
-      <c r="M13" s="63"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="167"/>
+      <c r="K13" s="64"/>
+      <c r="L13" s="167"/>
+      <c r="M13" s="167"/>
       <c r="N13" s="41"/>
       <c r="O13" s="40"/>
       <c r="P13" s="41"/>
@@ -25465,11 +25470,15 @@
       <c r="F14" s="73"/>
       <c r="G14" s="63"/>
       <c r="H14" s="8"/>
-      <c r="I14" s="142"/>
-      <c r="J14" s="141"/>
-      <c r="K14" s="145"/>
-      <c r="L14" s="141"/>
-      <c r="M14" s="81"/>
+      <c r="I14" s="164" t="s">
+        <v>296</v>
+      </c>
+      <c r="J14" s="166"/>
+      <c r="K14" s="144"/>
+      <c r="L14" s="164" t="s">
+        <v>297</v>
+      </c>
+      <c r="M14" s="166"/>
       <c r="N14" s="41"/>
       <c r="O14" s="40"/>
       <c r="P14" s="41"/>
@@ -25491,7 +25500,13 @@
       <c r="F15" s="78"/>
       <c r="G15" s="79"/>
       <c r="H15" s="8"/>
-      <c r="K15" s="143"/>
+      <c r="I15" s="126" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="139"/>
+      <c r="K15" s="145"/>
+      <c r="L15" s="138"/>
+      <c r="M15" s="76"/>
       <c r="N15" s="41"/>
       <c r="O15" s="40"/>
       <c r="P15" s="41"/>
@@ -25513,15 +25528,13 @@
       <c r="F16" s="73"/>
       <c r="G16" s="63"/>
       <c r="H16" s="8"/>
-      <c r="I16" s="164" t="s">
-        <v>296</v>
-      </c>
-      <c r="J16" s="165"/>
-      <c r="K16" s="144"/>
-      <c r="L16" s="165" t="s">
-        <v>297</v>
-      </c>
-      <c r="M16" s="166"/>
+      <c r="I16" s="117" t="s">
+        <v>312</v>
+      </c>
+      <c r="J16" s="140"/>
+      <c r="K16" s="145"/>
+      <c r="L16" s="105"/>
+      <c r="M16" s="63"/>
       <c r="N16" s="41"/>
       <c r="O16" s="40"/>
       <c r="P16" s="41"/>
@@ -25543,13 +25556,13 @@
       <c r="F17" s="146"/>
       <c r="G17" s="81"/>
       <c r="H17" s="8"/>
-      <c r="I17" s="126" t="s">
-        <v>26</v>
+      <c r="I17" s="116" t="s">
+        <v>309</v>
       </c>
       <c r="J17" s="139"/>
       <c r="K17" s="145"/>
-      <c r="L17" s="138"/>
-      <c r="M17" s="76"/>
+      <c r="L17" s="77"/>
+      <c r="M17" s="79"/>
       <c r="N17" s="41"/>
       <c r="O17" s="40"/>
       <c r="P17" s="41"/>
@@ -25569,12 +25582,10 @@
       <c r="F18" s="31"/>
       <c r="G18" s="64"/>
       <c r="H18" s="8"/>
-      <c r="I18" s="117" t="s">
-        <v>312</v>
-      </c>
+      <c r="I18" s="117"/>
       <c r="J18" s="140"/>
       <c r="K18" s="145"/>
-      <c r="L18" s="105"/>
+      <c r="L18" s="57"/>
       <c r="M18" s="63"/>
       <c r="N18" s="41"/>
       <c r="O18" s="40"/>
@@ -25595,13 +25606,11 @@
       <c r="F19" s="31"/>
       <c r="G19" s="64"/>
       <c r="H19" s="8"/>
-      <c r="I19" s="116" t="s">
-        <v>309</v>
-      </c>
-      <c r="J19" s="139"/>
+      <c r="I19" s="142"/>
+      <c r="J19" s="141"/>
       <c r="K19" s="145"/>
-      <c r="L19" s="77"/>
-      <c r="M19" s="79"/>
+      <c r="L19" s="141"/>
+      <c r="M19" s="81"/>
       <c r="N19" s="41"/>
       <c r="O19" s="40"/>
       <c r="P19" s="41"/>
@@ -25621,11 +25630,7 @@
       <c r="F20" s="31"/>
       <c r="G20" s="64"/>
       <c r="H20" s="8"/>
-      <c r="I20" s="117"/>
-      <c r="J20" s="140"/>
-      <c r="K20" s="145"/>
-      <c r="L20" s="57"/>
-      <c r="M20" s="63"/>
+      <c r="K20" s="143"/>
       <c r="N20" s="41"/>
       <c r="O20" s="40"/>
       <c r="P20" s="41"/>
@@ -25645,11 +25650,15 @@
       <c r="F21" s="31"/>
       <c r="G21" s="64"/>
       <c r="H21" s="8"/>
-      <c r="I21" s="142"/>
-      <c r="J21" s="141"/>
-      <c r="K21" s="145"/>
-      <c r="L21" s="141"/>
-      <c r="M21" s="81"/>
+      <c r="I21" s="164" t="s">
+        <v>298</v>
+      </c>
+      <c r="J21" s="166"/>
+      <c r="K21" s="144"/>
+      <c r="L21" s="164" t="s">
+        <v>299</v>
+      </c>
+      <c r="M21" s="166"/>
       <c r="N21" s="41"/>
       <c r="O21" s="93" t="s">
         <v>32</v>
@@ -25679,7 +25688,11 @@
       <c r="F22" s="31"/>
       <c r="G22" s="64"/>
       <c r="H22" s="8"/>
-      <c r="K22" s="143"/>
+      <c r="I22" s="126"/>
+      <c r="J22" s="139"/>
+      <c r="K22" s="145"/>
+      <c r="L22" s="138"/>
+      <c r="M22" s="76"/>
       <c r="N22" s="41"/>
       <c r="O22" s="67" t="s">
         <v>33</v>
@@ -25711,15 +25724,11 @@
       <c r="F23" s="31"/>
       <c r="G23" s="64"/>
       <c r="H23" s="8"/>
-      <c r="I23" s="164" t="s">
-        <v>298</v>
-      </c>
-      <c r="J23" s="165"/>
-      <c r="K23" s="144"/>
-      <c r="L23" s="165" t="s">
-        <v>299</v>
-      </c>
-      <c r="M23" s="166"/>
+      <c r="I23" s="117"/>
+      <c r="J23" s="140"/>
+      <c r="K23" s="145"/>
+      <c r="L23" s="105"/>
+      <c r="M23" s="63"/>
       <c r="N23" s="41"/>
       <c r="O23" s="98" t="s">
         <v>34</v>
@@ -25751,11 +25760,11 @@
       <c r="F24" s="31"/>
       <c r="G24" s="64"/>
       <c r="H24" s="40"/>
-      <c r="I24" s="126"/>
+      <c r="I24" s="116"/>
       <c r="J24" s="139"/>
       <c r="K24" s="145"/>
-      <c r="L24" s="138"/>
-      <c r="M24" s="76"/>
+      <c r="L24" s="77"/>
+      <c r="M24" s="79"/>
       <c r="N24" s="41"/>
       <c r="O24" s="97" t="s">
         <v>35</v>
@@ -25773,7 +25782,7 @@
       </c>
       <c r="S24" s="41"/>
       <c r="T24" s="103" t="s">
-        <v>310</v>
+        <v>14</v>
       </c>
       <c r="U24" s="41"/>
       <c r="V24" s="41"/>
@@ -25790,7 +25799,7 @@
       <c r="I25" s="117"/>
       <c r="J25" s="140"/>
       <c r="K25" s="145"/>
-      <c r="L25" s="105"/>
+      <c r="L25" s="57"/>
       <c r="M25" s="63"/>
       <c r="N25" s="41"/>
       <c r="O25" s="98" t="s">
@@ -25808,7 +25817,9 @@
         <v>1.963888888888889</v>
       </c>
       <c r="S25" s="41"/>
-      <c r="T25" s="102"/>
+      <c r="T25" s="102" t="s">
+        <v>310</v>
+      </c>
       <c r="U25" s="41"/>
       <c r="V25" s="41"/>
     </row>
@@ -25821,11 +25832,11 @@
       <c r="F26" s="31"/>
       <c r="G26" s="64"/>
       <c r="H26" s="41"/>
-      <c r="I26" s="116"/>
-      <c r="J26" s="139"/>
+      <c r="I26" s="142"/>
+      <c r="J26" s="141"/>
       <c r="K26" s="145"/>
-      <c r="L26" s="77"/>
-      <c r="M26" s="79"/>
+      <c r="L26" s="141"/>
+      <c r="M26" s="81"/>
       <c r="N26" s="41"/>
       <c r="O26" s="97" t="s">
         <v>37</v>
@@ -25847,11 +25858,7 @@
       <c r="F27" s="31"/>
       <c r="G27" s="64"/>
       <c r="H27" s="41"/>
-      <c r="I27" s="117"/>
-      <c r="J27" s="140"/>
-      <c r="K27" s="145"/>
-      <c r="L27" s="57"/>
-      <c r="M27" s="63"/>
+      <c r="K27" s="143"/>
       <c r="N27" s="41"/>
       <c r="O27" s="98" t="s">
         <v>38</v>
@@ -25873,11 +25880,15 @@
       <c r="F28" s="31"/>
       <c r="G28" s="64"/>
       <c r="H28" s="41"/>
-      <c r="I28" s="142"/>
-      <c r="J28" s="141"/>
-      <c r="K28" s="145"/>
-      <c r="L28" s="141"/>
-      <c r="M28" s="81"/>
+      <c r="I28" s="164" t="s">
+        <v>300</v>
+      </c>
+      <c r="J28" s="166"/>
+      <c r="K28" s="144"/>
+      <c r="L28" s="164" t="s">
+        <v>301</v>
+      </c>
+      <c r="M28" s="166"/>
       <c r="N28" s="41"/>
       <c r="O28" s="97" t="s">
         <v>39</v>
@@ -25899,7 +25910,11 @@
       <c r="F29" s="31"/>
       <c r="G29" s="64"/>
       <c r="H29" s="41"/>
-      <c r="K29" s="143"/>
+      <c r="I29" s="126"/>
+      <c r="J29" s="139"/>
+      <c r="K29" s="145"/>
+      <c r="L29" s="138"/>
+      <c r="M29" s="76"/>
       <c r="N29" s="41"/>
       <c r="O29" s="98" t="s">
         <v>40</v>
@@ -25921,15 +25936,11 @@
       <c r="F30" s="31"/>
       <c r="G30" s="64"/>
       <c r="H30" s="41"/>
-      <c r="I30" s="164" t="s">
-        <v>300</v>
-      </c>
-      <c r="J30" s="165"/>
-      <c r="K30" s="144"/>
-      <c r="L30" s="165" t="s">
-        <v>301</v>
-      </c>
-      <c r="M30" s="166"/>
+      <c r="I30" s="117"/>
+      <c r="J30" s="140"/>
+      <c r="K30" s="145"/>
+      <c r="L30" s="105"/>
+      <c r="M30" s="63"/>
       <c r="N30" s="41"/>
       <c r="O30" s="97" t="s">
         <v>41</v>
@@ -25951,11 +25962,11 @@
       <c r="F31" s="31"/>
       <c r="G31" s="64"/>
       <c r="H31" s="41"/>
-      <c r="I31" s="126"/>
+      <c r="I31" s="116"/>
       <c r="J31" s="139"/>
       <c r="K31" s="145"/>
-      <c r="L31" s="138"/>
-      <c r="M31" s="76"/>
+      <c r="L31" s="77"/>
+      <c r="M31" s="79"/>
       <c r="N31" s="41"/>
       <c r="O31" s="98" t="s">
         <v>42</v>
@@ -25980,7 +25991,7 @@
       <c r="I32" s="117"/>
       <c r="J32" s="140"/>
       <c r="K32" s="145"/>
-      <c r="L32" s="105"/>
+      <c r="L32" s="57"/>
       <c r="M32" s="63"/>
       <c r="N32" s="41"/>
       <c r="O32" s="97" t="s">
@@ -26003,11 +26014,11 @@
       <c r="F33" s="31"/>
       <c r="G33" s="64"/>
       <c r="H33" s="41"/>
-      <c r="I33" s="116"/>
-      <c r="J33" s="139"/>
+      <c r="I33" s="142"/>
+      <c r="J33" s="141"/>
       <c r="K33" s="145"/>
-      <c r="L33" s="77"/>
-      <c r="M33" s="79"/>
+      <c r="L33" s="141"/>
+      <c r="M33" s="81"/>
       <c r="N33" s="41"/>
       <c r="O33" s="98" t="s">
         <v>44</v>
@@ -26031,11 +26042,7 @@
       <c r="F34" s="31"/>
       <c r="G34" s="64"/>
       <c r="H34" s="41"/>
-      <c r="I34" s="117"/>
-      <c r="J34" s="140"/>
-      <c r="K34" s="145"/>
-      <c r="L34" s="57"/>
-      <c r="M34" s="63"/>
+      <c r="K34" s="143"/>
       <c r="N34" s="41"/>
       <c r="O34" s="130" t="s">
         <v>83</v>
@@ -26066,11 +26073,15 @@
       <c r="F35" s="31"/>
       <c r="G35" s="64"/>
       <c r="H35" s="41"/>
-      <c r="I35" s="142"/>
-      <c r="J35" s="141"/>
-      <c r="K35" s="145"/>
-      <c r="L35" s="141"/>
-      <c r="M35" s="81"/>
+      <c r="I35" s="164" t="s">
+        <v>302</v>
+      </c>
+      <c r="J35" s="166"/>
+      <c r="K35" s="144"/>
+      <c r="L35" s="164" t="s">
+        <v>303</v>
+      </c>
+      <c r="M35" s="166"/>
       <c r="N35" s="41"/>
       <c r="O35" s="41"/>
       <c r="P35" s="41"/>
@@ -26090,11 +26101,15 @@
       <c r="F36" s="31"/>
       <c r="G36" s="64"/>
       <c r="H36" s="41"/>
-      <c r="K36" s="143"/>
+      <c r="I36" s="126"/>
+      <c r="J36" s="139"/>
+      <c r="K36" s="145"/>
+      <c r="L36" s="138"/>
+      <c r="M36" s="76"/>
       <c r="N36" s="41"/>
-      <c r="O36" s="163"/>
-      <c r="P36" s="163"/>
-      <c r="Q36" s="163"/>
+      <c r="O36" s="157"/>
+      <c r="P36" s="157"/>
+      <c r="Q36" s="157"/>
       <c r="R36" s="129"/>
       <c r="S36" s="43"/>
       <c r="T36" s="43"/>
@@ -26110,19 +26125,15 @@
       <c r="F37" s="31"/>
       <c r="G37" s="64"/>
       <c r="H37" s="41"/>
-      <c r="I37" s="164" t="s">
-        <v>302</v>
-      </c>
-      <c r="J37" s="165"/>
-      <c r="K37" s="144"/>
-      <c r="L37" s="165" t="s">
-        <v>303</v>
-      </c>
-      <c r="M37" s="166"/>
+      <c r="I37" s="117"/>
+      <c r="J37" s="140"/>
+      <c r="K37" s="145"/>
+      <c r="L37" s="105"/>
+      <c r="M37" s="63"/>
       <c r="N37" s="41"/>
-      <c r="O37" s="163"/>
-      <c r="P37" s="163"/>
-      <c r="Q37" s="163"/>
+      <c r="O37" s="157"/>
+      <c r="P37" s="157"/>
+      <c r="Q37" s="157"/>
       <c r="R37" s="129"/>
       <c r="S37" s="43"/>
       <c r="T37" s="43"/>
@@ -26138,15 +26149,15 @@
       <c r="F38" s="31"/>
       <c r="G38" s="64"/>
       <c r="H38" s="41"/>
-      <c r="I38" s="126"/>
+      <c r="I38" s="116"/>
       <c r="J38" s="139"/>
       <c r="K38" s="145"/>
-      <c r="L38" s="138"/>
-      <c r="M38" s="76"/>
+      <c r="L38" s="77"/>
+      <c r="M38" s="79"/>
       <c r="N38" s="41"/>
-      <c r="O38" s="163"/>
-      <c r="P38" s="163"/>
-      <c r="Q38" s="163"/>
+      <c r="O38" s="157"/>
+      <c r="P38" s="157"/>
+      <c r="Q38" s="157"/>
       <c r="R38" s="129"/>
       <c r="S38" s="43"/>
       <c r="T38" s="43"/>
@@ -26165,12 +26176,12 @@
       <c r="I39" s="117"/>
       <c r="J39" s="140"/>
       <c r="K39" s="145"/>
-      <c r="L39" s="105"/>
+      <c r="L39" s="57"/>
       <c r="M39" s="63"/>
       <c r="N39" s="41"/>
-      <c r="O39" s="163"/>
-      <c r="P39" s="163"/>
-      <c r="Q39" s="163"/>
+      <c r="O39" s="157"/>
+      <c r="P39" s="157"/>
+      <c r="Q39" s="157"/>
       <c r="R39" s="128"/>
       <c r="S39" s="43"/>
       <c r="T39" s="43"/>
@@ -26186,15 +26197,15 @@
       <c r="F40" s="40"/>
       <c r="G40" s="65"/>
       <c r="H40" s="41"/>
-      <c r="I40" s="116"/>
-      <c r="J40" s="139"/>
+      <c r="I40" s="142"/>
+      <c r="J40" s="141"/>
       <c r="K40" s="145"/>
-      <c r="L40" s="77"/>
-      <c r="M40" s="79"/>
+      <c r="L40" s="141"/>
+      <c r="M40" s="81"/>
       <c r="N40" s="41"/>
-      <c r="O40" s="163"/>
-      <c r="P40" s="163"/>
-      <c r="Q40" s="163"/>
+      <c r="O40" s="157"/>
+      <c r="P40" s="157"/>
+      <c r="Q40" s="157"/>
       <c r="R40" s="128"/>
       <c r="S40" s="43"/>
       <c r="T40" s="43"/>
@@ -26210,15 +26221,10 @@
       <c r="F41" s="31"/>
       <c r="G41" s="64"/>
       <c r="H41" s="41"/>
-      <c r="I41" s="117"/>
-      <c r="J41" s="140"/>
-      <c r="K41" s="145"/>
-      <c r="L41" s="57"/>
-      <c r="M41" s="63"/>
       <c r="N41" s="41"/>
-      <c r="O41" s="163"/>
-      <c r="P41" s="163"/>
-      <c r="Q41" s="163"/>
+      <c r="O41" s="157"/>
+      <c r="P41" s="157"/>
+      <c r="Q41" s="157"/>
       <c r="R41" s="128"/>
       <c r="S41" s="43"/>
       <c r="T41" s="43"/>
@@ -26234,11 +26240,6 @@
       <c r="F42" s="31"/>
       <c r="G42" s="64"/>
       <c r="H42" s="41"/>
-      <c r="I42" s="142"/>
-      <c r="J42" s="141"/>
-      <c r="K42" s="145"/>
-      <c r="L42" s="141"/>
-      <c r="M42" s="81"/>
       <c r="N42" s="41"/>
       <c r="O42" s="40"/>
       <c r="P42" s="40"/>
@@ -29066,24 +29067,24 @@
     <sortCondition ref="I9"/>
   </sortState>
   <mergeCells count="18">
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="I35:J35"/>
     <mergeCell ref="O41:Q41"/>
     <mergeCell ref="O36:Q36"/>
     <mergeCell ref="O37:Q37"/>
     <mergeCell ref="O38:Q38"/>
     <mergeCell ref="O39:Q39"/>
     <mergeCell ref="O40:Q40"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="L16:M16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I116" r:id="rId1"/>

</xml_diff>

<commit_message>
Just finished 13 Sentinels!
What an experience
</commit_message>
<xml_diff>
--- a/spreadsheets/Games.xlsx
+++ b/spreadsheets/Games.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="317">
   <si>
     <t>Nier: Automata</t>
   </si>
@@ -1329,6 +1329,12 @@
   </si>
   <si>
     <t>9-oct.</t>
+  </si>
+  <si>
+    <t>10-may.</t>
+  </si>
+  <si>
+    <t>13 Sentinels (14h 55m)</t>
   </si>
 </sst>
 </file>
@@ -2132,6 +2138,9 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2162,9 +2171,6 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
@@ -2183,16 +2189,16 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2717,11 +2723,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1381972208"/>
-        <c:axId val="-1381968944"/>
+        <c:axId val="316192880"/>
+        <c:axId val="316187440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1381972208"/>
+        <c:axId val="316192880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2802,7 +2808,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1381968944"/>
+        <c:crossAx val="316187440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2810,7 +2816,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1381968944"/>
+        <c:axId val="316187440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2912,7 +2918,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1381972208"/>
+        <c:crossAx val="316192880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3284,11 +3290,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1381976016"/>
-        <c:axId val="-1381971664"/>
+        <c:axId val="316193424"/>
+        <c:axId val="316194512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1381976016"/>
+        <c:axId val="316193424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3331,7 +3337,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1381971664"/>
+        <c:crossAx val="316194512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3339,7 +3345,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1381971664"/>
+        <c:axId val="316194512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3390,7 +3396,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1381976016"/>
+        <c:crossAx val="316193424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3777,11 +3783,11 @@
         </c:dLbls>
         <c:gapWidth val="444"/>
         <c:overlap val="-90"/>
-        <c:axId val="-1381969488"/>
-        <c:axId val="-1381968400"/>
+        <c:axId val="316197232"/>
+        <c:axId val="316190160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1381969488"/>
+        <c:axId val="316197232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3838,7 +3844,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1381968400"/>
+        <c:crossAx val="316190160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3846,7 +3852,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1381968400"/>
+        <c:axId val="316190160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3856,7 +3862,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1381969488"/>
+        <c:crossAx val="316197232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4170,11 +4176,11 @@
         </c:dLbls>
         <c:gapWidth val="50"/>
         <c:overlap val="100"/>
-        <c:axId val="-1186767312"/>
-        <c:axId val="-1186756432"/>
+        <c:axId val="316195056"/>
+        <c:axId val="316188528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1186767312"/>
+        <c:axId val="316195056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4219,7 +4225,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1186756432"/>
+        <c:crossAx val="316188528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4227,7 +4233,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1186756432"/>
+        <c:axId val="316188528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4277,7 +4283,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1186767312"/>
+        <c:crossAx val="316195056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.5"/>
@@ -4300,7 +4306,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4415,7 +4420,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4505,7 +4509,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4715,11 +4718,11 @@
         </c:dLbls>
         <c:gapWidth val="444"/>
         <c:overlap val="-90"/>
-        <c:axId val="-1186771120"/>
-        <c:axId val="-1186758608"/>
+        <c:axId val="316189072"/>
+        <c:axId val="316191792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1186771120"/>
+        <c:axId val="316189072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4776,7 +4779,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1186758608"/>
+        <c:crossAx val="316191792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4784,7 +4787,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1186758608"/>
+        <c:axId val="316191792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4794,7 +4797,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1186771120"/>
+        <c:crossAx val="316189072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5060,11 +5063,11 @@
         </c:dLbls>
         <c:gapWidth val="50"/>
         <c:overlap val="100"/>
-        <c:axId val="-1186760240"/>
-        <c:axId val="-1186757520"/>
+        <c:axId val="316185808"/>
+        <c:axId val="316189616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1186760240"/>
+        <c:axId val="316185808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5109,7 +5112,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1186757520"/>
+        <c:crossAx val="316189616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5117,7 +5120,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1186757520"/>
+        <c:axId val="316189616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5167,7 +5170,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1186760240"/>
+        <c:crossAx val="316185808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.5"/>
@@ -9140,17 +9143,17 @@
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="147">
+      <c r="B2" s="148">
         <v>2019</v>
       </c>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
+      <c r="C2" s="149"/>
+      <c r="D2" s="149"/>
       <c r="E2" s="71"/>
-      <c r="F2" s="153" t="s">
+      <c r="F2" s="154" t="s">
         <v>269</v>
       </c>
-      <c r="G2" s="153"/>
-      <c r="H2" s="153"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
       <c r="I2" s="36"/>
       <c r="J2" s="36"/>
       <c r="K2" s="36"/>
@@ -9181,18 +9184,18 @@
         <v>83</v>
       </c>
       <c r="E3" s="72"/>
-      <c r="F3" s="153"/>
-      <c r="G3" s="153"/>
-      <c r="H3" s="153"/>
+      <c r="F3" s="154"/>
+      <c r="G3" s="154"/>
+      <c r="H3" s="154"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
       <c r="M3" s="8"/>
       <c r="N3" s="30"/>
-      <c r="O3" s="152"/>
-      <c r="P3" s="152"/>
-      <c r="Q3" s="152"/>
+      <c r="O3" s="153"/>
+      <c r="P3" s="153"/>
+      <c r="Q3" s="153"/>
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
@@ -9214,18 +9217,18 @@
         <v>2004</v>
       </c>
       <c r="E4" s="27"/>
-      <c r="F4" s="153"/>
-      <c r="G4" s="153"/>
-      <c r="H4" s="153"/>
+      <c r="F4" s="154"/>
+      <c r="G4" s="154"/>
+      <c r="H4" s="154"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="31"/>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="7"/>
-      <c r="O4" s="152"/>
-      <c r="P4" s="152"/>
-      <c r="Q4" s="152"/>
+      <c r="O4" s="153"/>
+      <c r="P4" s="153"/>
+      <c r="Q4" s="153"/>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
       <c r="T4" s="6"/>
@@ -9247,18 +9250,18 @@
         <v>2017</v>
       </c>
       <c r="E5" s="27"/>
-      <c r="F5" s="153"/>
-      <c r="G5" s="153"/>
-      <c r="H5" s="153"/>
+      <c r="F5" s="154"/>
+      <c r="G5" s="154"/>
+      <c r="H5" s="154"/>
       <c r="I5" s="8"/>
       <c r="J5" s="31"/>
       <c r="K5" s="31"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="7"/>
-      <c r="O5" s="152"/>
-      <c r="P5" s="152"/>
-      <c r="Q5" s="152"/>
+      <c r="O5" s="153"/>
+      <c r="P5" s="153"/>
+      <c r="Q5" s="153"/>
       <c r="R5" s="6"/>
       <c r="S5" s="6"/>
       <c r="T5" s="6"/>
@@ -9280,18 +9283,18 @@
         <v>2017</v>
       </c>
       <c r="E6" s="27"/>
-      <c r="F6" s="153"/>
-      <c r="G6" s="153"/>
-      <c r="H6" s="153"/>
+      <c r="F6" s="154"/>
+      <c r="G6" s="154"/>
+      <c r="H6" s="154"/>
       <c r="I6" s="8"/>
       <c r="J6" s="31"/>
       <c r="K6" s="31"/>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="7"/>
-      <c r="O6" s="152"/>
-      <c r="P6" s="152"/>
-      <c r="Q6" s="152"/>
+      <c r="O6" s="153"/>
+      <c r="P6" s="153"/>
+      <c r="Q6" s="153"/>
       <c r="R6" s="6"/>
       <c r="S6" s="6"/>
       <c r="T6" s="6"/>
@@ -9313,18 +9316,18 @@
         <v>2017</v>
       </c>
       <c r="E7" s="27"/>
-      <c r="F7" s="153"/>
-      <c r="G7" s="153"/>
-      <c r="H7" s="153"/>
+      <c r="F7" s="154"/>
+      <c r="G7" s="154"/>
+      <c r="H7" s="154"/>
       <c r="I7" s="8"/>
       <c r="J7" s="31"/>
       <c r="K7" s="31"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="7"/>
-      <c r="O7" s="152"/>
-      <c r="P7" s="152"/>
-      <c r="Q7" s="152"/>
+      <c r="O7" s="153"/>
+      <c r="P7" s="153"/>
+      <c r="Q7" s="153"/>
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
       <c r="T7" s="6"/>
@@ -9346,18 +9349,18 @@
         <v>2017</v>
       </c>
       <c r="E8" s="27"/>
-      <c r="F8" s="153"/>
-      <c r="G8" s="153"/>
-      <c r="H8" s="153"/>
+      <c r="F8" s="154"/>
+      <c r="G8" s="154"/>
+      <c r="H8" s="154"/>
       <c r="I8" s="8"/>
       <c r="J8" s="31"/>
       <c r="K8" s="31"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="7"/>
-      <c r="O8" s="152"/>
-      <c r="P8" s="152"/>
-      <c r="Q8" s="152"/>
+      <c r="O8" s="153"/>
+      <c r="P8" s="153"/>
+      <c r="Q8" s="153"/>
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
@@ -9379,18 +9382,18 @@
         <v>2016</v>
       </c>
       <c r="E9" s="27"/>
-      <c r="F9" s="153"/>
-      <c r="G9" s="153"/>
-      <c r="H9" s="153"/>
+      <c r="F9" s="154"/>
+      <c r="G9" s="154"/>
+      <c r="H9" s="154"/>
       <c r="I9" s="8"/>
       <c r="J9" s="31"/>
       <c r="K9" s="31"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="7"/>
-      <c r="O9" s="152"/>
-      <c r="P9" s="152"/>
-      <c r="Q9" s="152"/>
+      <c r="O9" s="153"/>
+      <c r="P9" s="153"/>
+      <c r="Q9" s="153"/>
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
@@ -9412,18 +9415,18 @@
         <v>2017</v>
       </c>
       <c r="E10" s="27"/>
-      <c r="F10" s="153"/>
-      <c r="G10" s="153"/>
-      <c r="H10" s="153"/>
+      <c r="F10" s="154"/>
+      <c r="G10" s="154"/>
+      <c r="H10" s="154"/>
       <c r="I10" s="8"/>
       <c r="J10" s="31"/>
       <c r="K10" s="31"/>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="7"/>
-      <c r="O10" s="152"/>
-      <c r="P10" s="152"/>
-      <c r="Q10" s="152"/>
+      <c r="O10" s="153"/>
+      <c r="P10" s="153"/>
+      <c r="Q10" s="153"/>
       <c r="R10" s="6"/>
       <c r="S10" s="6"/>
       <c r="T10" s="6"/>
@@ -9445,18 +9448,18 @@
         <v>2016</v>
       </c>
       <c r="E11" s="27"/>
-      <c r="F11" s="153"/>
-      <c r="G11" s="153"/>
-      <c r="H11" s="153"/>
+      <c r="F11" s="154"/>
+      <c r="G11" s="154"/>
+      <c r="H11" s="154"/>
       <c r="I11" s="8"/>
       <c r="J11" s="31"/>
       <c r="K11" s="31"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="7"/>
-      <c r="O11" s="152"/>
-      <c r="P11" s="152"/>
-      <c r="Q11" s="152"/>
+      <c r="O11" s="153"/>
+      <c r="P11" s="153"/>
+      <c r="Q11" s="153"/>
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
@@ -9478,18 +9481,18 @@
         <v>2017</v>
       </c>
       <c r="E12" s="27"/>
-      <c r="F12" s="153"/>
-      <c r="G12" s="153"/>
-      <c r="H12" s="153"/>
+      <c r="F12" s="154"/>
+      <c r="G12" s="154"/>
+      <c r="H12" s="154"/>
       <c r="I12" s="8"/>
       <c r="J12" s="31"/>
       <c r="K12" s="31"/>
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="7"/>
-      <c r="O12" s="152"/>
-      <c r="P12" s="152"/>
-      <c r="Q12" s="152"/>
+      <c r="O12" s="153"/>
+      <c r="P12" s="153"/>
+      <c r="Q12" s="153"/>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
@@ -9511,18 +9514,18 @@
         <v>2009</v>
       </c>
       <c r="E13" s="27"/>
-      <c r="F13" s="153"/>
-      <c r="G13" s="153"/>
-      <c r="H13" s="153"/>
+      <c r="F13" s="154"/>
+      <c r="G13" s="154"/>
+      <c r="H13" s="154"/>
       <c r="I13" s="8"/>
       <c r="J13" s="31"/>
       <c r="K13" s="31"/>
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="7"/>
-      <c r="O13" s="152"/>
-      <c r="P13" s="152"/>
-      <c r="Q13" s="152"/>
+      <c r="O13" s="153"/>
+      <c r="P13" s="153"/>
+      <c r="Q13" s="153"/>
       <c r="R13" s="6"/>
       <c r="S13" s="6"/>
       <c r="T13" s="6"/>
@@ -9544,18 +9547,18 @@
         <v>2019</v>
       </c>
       <c r="E14" s="27"/>
-      <c r="F14" s="153"/>
-      <c r="G14" s="153"/>
-      <c r="H14" s="153"/>
+      <c r="F14" s="154"/>
+      <c r="G14" s="154"/>
+      <c r="H14" s="154"/>
       <c r="I14" s="8"/>
       <c r="J14" s="31"/>
       <c r="K14" s="31"/>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="7"/>
-      <c r="O14" s="152"/>
-      <c r="P14" s="152"/>
-      <c r="Q14" s="152"/>
+      <c r="O14" s="153"/>
+      <c r="P14" s="153"/>
+      <c r="Q14" s="153"/>
       <c r="R14" s="6"/>
       <c r="S14" s="6"/>
       <c r="T14" s="6"/>
@@ -9577,18 +9580,18 @@
         <v>2019</v>
       </c>
       <c r="E15" s="27"/>
-      <c r="F15" s="153"/>
-      <c r="G15" s="153"/>
-      <c r="H15" s="153"/>
+      <c r="F15" s="154"/>
+      <c r="G15" s="154"/>
+      <c r="H15" s="154"/>
       <c r="I15" s="8"/>
       <c r="J15" s="31"/>
       <c r="K15" s="31"/>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="7"/>
-      <c r="O15" s="152"/>
-      <c r="P15" s="152"/>
-      <c r="Q15" s="152"/>
+      <c r="O15" s="153"/>
+      <c r="P15" s="153"/>
+      <c r="Q15" s="153"/>
       <c r="R15" s="6"/>
       <c r="S15" s="6"/>
       <c r="T15" s="6"/>
@@ -9613,9 +9616,9 @@
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
-      <c r="O16" s="152"/>
-      <c r="P16" s="152"/>
-      <c r="Q16" s="152"/>
+      <c r="O16" s="153"/>
+      <c r="P16" s="153"/>
+      <c r="Q16" s="153"/>
       <c r="S16" s="6"/>
       <c r="T16" s="6"/>
       <c r="U16" s="6"/>
@@ -9626,9 +9629,9 @@
     </row>
     <row r="17" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
-      <c r="B17" s="149"/>
-      <c r="C17" s="149"/>
-      <c r="D17" s="149"/>
+      <c r="B17" s="150"/>
+      <c r="C17" s="150"/>
+      <c r="D17" s="150"/>
       <c r="E17" s="6"/>
       <c r="F17" s="8"/>
       <c r="G17" s="7"/>
@@ -9653,9 +9656,9 @@
     </row>
     <row r="18" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24"/>
-      <c r="B18" s="149"/>
-      <c r="C18" s="149"/>
-      <c r="D18" s="149"/>
+      <c r="B18" s="150"/>
+      <c r="C18" s="150"/>
+      <c r="D18" s="150"/>
       <c r="E18" s="6"/>
       <c r="F18" s="8"/>
       <c r="G18" s="7"/>
@@ -9665,8 +9668,8 @@
       <c r="K18" s="31"/>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
-      <c r="N18" s="150"/>
-      <c r="O18" s="151"/>
+      <c r="N18" s="151"/>
+      <c r="O18" s="152"/>
       <c r="P18" s="8"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
@@ -9680,9 +9683,9 @@
     </row>
     <row r="19" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="24"/>
-      <c r="B19" s="149"/>
-      <c r="C19" s="149"/>
-      <c r="D19" s="149"/>
+      <c r="B19" s="150"/>
+      <c r="C19" s="150"/>
+      <c r="D19" s="150"/>
       <c r="E19" s="6"/>
       <c r="F19" s="8"/>
       <c r="G19" s="7"/>
@@ -9692,8 +9695,8 @@
       <c r="K19" s="31"/>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
-      <c r="N19" s="151"/>
-      <c r="O19" s="151"/>
+      <c r="N19" s="152"/>
+      <c r="O19" s="152"/>
       <c r="P19" s="8"/>
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
@@ -9719,8 +9722,8 @@
       <c r="K20" s="31"/>
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
-      <c r="N20" s="151"/>
-      <c r="O20" s="151"/>
+      <c r="N20" s="152"/>
+      <c r="O20" s="152"/>
       <c r="P20" s="8"/>
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
@@ -9746,8 +9749,8 @@
       <c r="K21" s="31"/>
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
-      <c r="N21" s="151"/>
-      <c r="O21" s="151"/>
+      <c r="N21" s="152"/>
+      <c r="O21" s="152"/>
       <c r="P21" s="8"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
@@ -9773,8 +9776,8 @@
       <c r="K22" s="31"/>
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
-      <c r="N22" s="151"/>
-      <c r="O22" s="151"/>
+      <c r="N22" s="152"/>
+      <c r="O22" s="152"/>
       <c r="P22" s="8"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
@@ -10958,8 +10961,8 @@
         <v>11</v>
       </c>
       <c r="I17" s="8"/>
-      <c r="J17" s="155"/>
-      <c r="K17" s="156"/>
+      <c r="J17" s="156"/>
+      <c r="K17" s="157"/>
       <c r="L17" s="8"/>
       <c r="M17" s="40"/>
       <c r="N17" s="41"/>
@@ -10997,8 +11000,8 @@
         <v>1</v>
       </c>
       <c r="I18" s="8"/>
-      <c r="J18" s="154"/>
-      <c r="K18" s="154"/>
+      <c r="J18" s="155"/>
+      <c r="K18" s="155"/>
       <c r="L18" s="8"/>
       <c r="M18" s="40"/>
       <c r="N18" s="41"/>
@@ -17681,9 +17684,9 @@
         <v>4.5138888888888888E-2</v>
       </c>
       <c r="L36" s="41"/>
-      <c r="M36" s="157"/>
-      <c r="N36" s="157"/>
-      <c r="O36" s="157"/>
+      <c r="M36" s="164"/>
+      <c r="N36" s="164"/>
+      <c r="O36" s="164"/>
       <c r="P36" s="129"/>
       <c r="Q36" s="43"/>
       <c r="R36" s="43"/>
@@ -17750,9 +17753,9 @@
         <v>7.7777777777777779E-2</v>
       </c>
       <c r="L37" s="41"/>
-      <c r="M37" s="157"/>
-      <c r="N37" s="157"/>
-      <c r="O37" s="157"/>
+      <c r="M37" s="164"/>
+      <c r="N37" s="164"/>
+      <c r="O37" s="164"/>
       <c r="P37" s="129"/>
       <c r="Q37" s="43"/>
       <c r="R37" s="43"/>
@@ -17819,9 +17822,9 @@
         <v>9.1666666666666674E-2</v>
       </c>
       <c r="L38" s="41"/>
-      <c r="M38" s="157"/>
-      <c r="N38" s="157"/>
-      <c r="O38" s="157"/>
+      <c r="M38" s="164"/>
+      <c r="N38" s="164"/>
+      <c r="O38" s="164"/>
       <c r="P38" s="129"/>
       <c r="Q38" s="43"/>
       <c r="R38" s="43"/>
@@ -17878,9 +17881,9 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="L39" s="41"/>
-      <c r="M39" s="157"/>
-      <c r="N39" s="157"/>
-      <c r="O39" s="157"/>
+      <c r="M39" s="164"/>
+      <c r="N39" s="164"/>
+      <c r="O39" s="164"/>
       <c r="P39" s="128"/>
       <c r="Q39" s="43"/>
       <c r="R39" s="43"/>
@@ -17935,9 +17938,9 @@
         <v>0.3666666666666667</v>
       </c>
       <c r="L40" s="41"/>
-      <c r="M40" s="157"/>
-      <c r="N40" s="157"/>
-      <c r="O40" s="157"/>
+      <c r="M40" s="164"/>
+      <c r="N40" s="164"/>
+      <c r="O40" s="164"/>
       <c r="P40" s="128"/>
       <c r="Q40" s="43"/>
       <c r="R40" s="43"/>
@@ -17991,9 +17994,9 @@
         <v>0.53333333333333333</v>
       </c>
       <c r="L41" s="41"/>
-      <c r="M41" s="157"/>
-      <c r="N41" s="157"/>
-      <c r="O41" s="157"/>
+      <c r="M41" s="164"/>
+      <c r="N41" s="164"/>
+      <c r="O41" s="164"/>
       <c r="P41" s="128"/>
       <c r="Q41" s="43"/>
       <c r="R41" s="43"/>
@@ -24899,6 +24902,12 @@
     <sortCondition ref="J33"/>
   </sortState>
   <mergeCells count="18">
+    <mergeCell ref="M41:O41"/>
+    <mergeCell ref="M40:O40"/>
+    <mergeCell ref="M37:O37"/>
+    <mergeCell ref="M36:O36"/>
+    <mergeCell ref="M38:O38"/>
+    <mergeCell ref="M39:O39"/>
     <mergeCell ref="I58:I63"/>
     <mergeCell ref="I54:I57"/>
     <mergeCell ref="I50:I53"/>
@@ -24911,12 +24920,6 @@
     <mergeCell ref="I32:I38"/>
     <mergeCell ref="I27:I31"/>
     <mergeCell ref="I14:I19"/>
-    <mergeCell ref="M41:O41"/>
-    <mergeCell ref="M40:O40"/>
-    <mergeCell ref="M37:O37"/>
-    <mergeCell ref="M36:O36"/>
-    <mergeCell ref="M38:O38"/>
-    <mergeCell ref="M39:O39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -24933,7 +24936,7 @@
   <dimension ref="A1:V153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -25002,12 +25005,12 @@
         <v>21</v>
       </c>
       <c r="H2" s="8"/>
-      <c r="I2" s="164" t="s">
+      <c r="I2" s="165" t="s">
         <v>292</v>
       </c>
-      <c r="J2" s="165"/>
+      <c r="J2" s="167"/>
       <c r="K2" s="144"/>
-      <c r="L2" s="165" t="s">
+      <c r="L2" s="167" t="s">
         <v>293</v>
       </c>
       <c r="M2" s="166"/>
@@ -25290,12 +25293,12 @@
         <v>0.20416666666666669</v>
       </c>
       <c r="H9" s="8"/>
-      <c r="I9" s="164" t="s">
+      <c r="I9" s="165" t="s">
         <v>294</v>
       </c>
-      <c r="J9" s="165"/>
+      <c r="J9" s="167"/>
       <c r="K9" s="144"/>
-      <c r="L9" s="165" t="s">
+      <c r="L9" s="167" t="s">
         <v>295</v>
       </c>
       <c r="M9" s="166"/>
@@ -25408,10 +25411,10 @@
         <v>308</v>
       </c>
       <c r="F12" s="73" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="63" t="s">
-        <v>14</v>
+        <v>315</v>
+      </c>
+      <c r="G12" s="63">
+        <v>1.6291666666666667</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="116"/>
@@ -25445,10 +25448,10 @@
       <c r="G13" s="79"/>
       <c r="H13" s="8"/>
       <c r="I13" s="55"/>
-      <c r="J13" s="167"/>
+      <c r="J13" s="147"/>
       <c r="K13" s="64"/>
-      <c r="L13" s="167"/>
-      <c r="M13" s="167"/>
+      <c r="L13" s="147"/>
+      <c r="M13" s="147"/>
       <c r="N13" s="41"/>
       <c r="O13" s="40"/>
       <c r="P13" s="41"/>
@@ -25470,12 +25473,12 @@
       <c r="F14" s="73"/>
       <c r="G14" s="63"/>
       <c r="H14" s="8"/>
-      <c r="I14" s="164" t="s">
+      <c r="I14" s="165" t="s">
         <v>296</v>
       </c>
       <c r="J14" s="166"/>
       <c r="K14" s="144"/>
-      <c r="L14" s="164" t="s">
+      <c r="L14" s="165" t="s">
         <v>297</v>
       </c>
       <c r="M14" s="166"/>
@@ -25650,12 +25653,12 @@
       <c r="F21" s="31"/>
       <c r="G21" s="64"/>
       <c r="H21" s="8"/>
-      <c r="I21" s="164" t="s">
+      <c r="I21" s="165" t="s">
         <v>298</v>
       </c>
       <c r="J21" s="166"/>
       <c r="K21" s="144"/>
-      <c r="L21" s="164" t="s">
+      <c r="L21" s="165" t="s">
         <v>299</v>
       </c>
       <c r="M21" s="166"/>
@@ -25845,7 +25848,9 @@
       <c r="Q26" s="85"/>
       <c r="R26" s="101"/>
       <c r="S26" s="41"/>
-      <c r="T26" s="104"/>
+      <c r="T26" s="103" t="s">
+        <v>316</v>
+      </c>
       <c r="U26" s="41"/>
       <c r="V26" s="41"/>
     </row>
@@ -25880,12 +25885,12 @@
       <c r="F28" s="31"/>
       <c r="G28" s="64"/>
       <c r="H28" s="41"/>
-      <c r="I28" s="164" t="s">
+      <c r="I28" s="165" t="s">
         <v>300</v>
       </c>
       <c r="J28" s="166"/>
       <c r="K28" s="144"/>
-      <c r="L28" s="164" t="s">
+      <c r="L28" s="165" t="s">
         <v>301</v>
       </c>
       <c r="M28" s="166"/>
@@ -26073,12 +26078,12 @@
       <c r="F35" s="31"/>
       <c r="G35" s="64"/>
       <c r="H35" s="41"/>
-      <c r="I35" s="164" t="s">
+      <c r="I35" s="165" t="s">
         <v>302</v>
       </c>
       <c r="J35" s="166"/>
       <c r="K35" s="144"/>
-      <c r="L35" s="164" t="s">
+      <c r="L35" s="165" t="s">
         <v>303</v>
       </c>
       <c r="M35" s="166"/>
@@ -26107,9 +26112,9 @@
       <c r="L36" s="138"/>
       <c r="M36" s="76"/>
       <c r="N36" s="41"/>
-      <c r="O36" s="157"/>
-      <c r="P36" s="157"/>
-      <c r="Q36" s="157"/>
+      <c r="O36" s="164"/>
+      <c r="P36" s="164"/>
+      <c r="Q36" s="164"/>
       <c r="R36" s="129"/>
       <c r="S36" s="43"/>
       <c r="T36" s="43"/>
@@ -26131,9 +26136,9 @@
       <c r="L37" s="105"/>
       <c r="M37" s="63"/>
       <c r="N37" s="41"/>
-      <c r="O37" s="157"/>
-      <c r="P37" s="157"/>
-      <c r="Q37" s="157"/>
+      <c r="O37" s="164"/>
+      <c r="P37" s="164"/>
+      <c r="Q37" s="164"/>
       <c r="R37" s="129"/>
       <c r="S37" s="43"/>
       <c r="T37" s="43"/>
@@ -26155,9 +26160,9 @@
       <c r="L38" s="77"/>
       <c r="M38" s="79"/>
       <c r="N38" s="41"/>
-      <c r="O38" s="157"/>
-      <c r="P38" s="157"/>
-      <c r="Q38" s="157"/>
+      <c r="O38" s="164"/>
+      <c r="P38" s="164"/>
+      <c r="Q38" s="164"/>
       <c r="R38" s="129"/>
       <c r="S38" s="43"/>
       <c r="T38" s="43"/>
@@ -26179,9 +26184,9 @@
       <c r="L39" s="57"/>
       <c r="M39" s="63"/>
       <c r="N39" s="41"/>
-      <c r="O39" s="157"/>
-      <c r="P39" s="157"/>
-      <c r="Q39" s="157"/>
+      <c r="O39" s="164"/>
+      <c r="P39" s="164"/>
+      <c r="Q39" s="164"/>
       <c r="R39" s="128"/>
       <c r="S39" s="43"/>
       <c r="T39" s="43"/>
@@ -26203,9 +26208,9 @@
       <c r="L40" s="141"/>
       <c r="M40" s="81"/>
       <c r="N40" s="41"/>
-      <c r="O40" s="157"/>
-      <c r="P40" s="157"/>
-      <c r="Q40" s="157"/>
+      <c r="O40" s="164"/>
+      <c r="P40" s="164"/>
+      <c r="Q40" s="164"/>
       <c r="R40" s="128"/>
       <c r="S40" s="43"/>
       <c r="T40" s="43"/>
@@ -26222,9 +26227,9 @@
       <c r="G41" s="64"/>
       <c r="H41" s="41"/>
       <c r="N41" s="41"/>
-      <c r="O41" s="157"/>
-      <c r="P41" s="157"/>
-      <c r="Q41" s="157"/>
+      <c r="O41" s="164"/>
+      <c r="P41" s="164"/>
+      <c r="Q41" s="164"/>
       <c r="R41" s="128"/>
       <c r="S41" s="43"/>
       <c r="T41" s="43"/>
@@ -29067,6 +29072,12 @@
     <sortCondition ref="I9"/>
   </sortState>
   <mergeCells count="18">
+    <mergeCell ref="O41:Q41"/>
+    <mergeCell ref="O36:Q36"/>
+    <mergeCell ref="O37:Q37"/>
+    <mergeCell ref="O38:Q38"/>
+    <mergeCell ref="O39:Q39"/>
+    <mergeCell ref="O40:Q40"/>
     <mergeCell ref="L35:M35"/>
     <mergeCell ref="L28:M28"/>
     <mergeCell ref="L21:M21"/>
@@ -29079,19 +29090,13 @@
     <mergeCell ref="L14:M14"/>
     <mergeCell ref="I28:J28"/>
     <mergeCell ref="I35:J35"/>
-    <mergeCell ref="O41:Q41"/>
-    <mergeCell ref="O36:Q36"/>
-    <mergeCell ref="O37:Q37"/>
-    <mergeCell ref="O38:Q38"/>
-    <mergeCell ref="O39:Q39"/>
-    <mergeCell ref="O40:Q40"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I116" r:id="rId1"/>
     <hyperlink ref="I117" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <ignoredErrors>
     <ignoredError sqref="Q146" formula="1"/>
   </ignoredErrors>

</xml_diff>